<commit_message>
lo que agregamos en la clase de practica
</commit_message>
<xml_diff>
--- a/tablas_ base de datos.xlsx
+++ b/tablas_ base de datos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr checkCompatibility="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="BASE DE DATOS" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="188">
   <si>
     <t>PRODUCTOS</t>
   </si>
@@ -601,12 +601,6 @@
     <t>genero</t>
   </si>
   <si>
-    <t>genero_id</t>
-  </si>
-  <si>
-    <t>producto_id</t>
-  </si>
-  <si>
     <r>
       <t>categorias_id</t>
     </r>
@@ -629,82 +623,12 @@
     <t>ver si aca llamo a categoria para poner que es indumentaria</t>
   </si>
   <si>
-    <r>
-      <t>producto_id</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(FK)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>genero_id</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(FK)</t>
-    </r>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
-    <t>talle_id</t>
-  </si>
-  <si>
-    <r>
-      <t>talle_id</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(FK)</t>
-    </r>
-  </si>
-  <si>
-    <t>categoria_id?</t>
-  </si>
-  <si>
     <t xml:space="preserve">lorem ipsum </t>
   </si>
   <si>
-    <r>
-      <t>categoria_id</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(FK)</t>
-    </r>
-  </si>
-  <si>
     <t>taza.jpg</t>
   </si>
   <si>
@@ -765,16 +689,7 @@
     <t>xio</t>
   </si>
   <si>
-    <t>VARCHAR(50)???</t>
-  </si>
-  <si>
-    <t>DATETIME???</t>
-  </si>
-  <si>
     <t xml:space="preserve"> confirmar si todos las claves foraneas de las tablas intermedias, tambien van ahi...</t>
-  </si>
-  <si>
-    <t>DATETIME??</t>
   </si>
   <si>
     <t>el principito</t>
@@ -1001,22 +916,6 @@
   </si>
   <si>
     <r>
-      <t>categoria_id</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(FK)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>product_id</t>
     </r>
     <r>
@@ -1130,7 +1029,181 @@
     <t>Type</t>
   </si>
   <si>
-    <t>CARRITO_PRODUCT</t>
+    <t>CART_PRODUCT</t>
+  </si>
+  <si>
+    <t>CARTS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">cart_id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>PRODUCT_SIZE</t>
+  </si>
+  <si>
+    <t>CONTRAINTS</t>
+  </si>
+  <si>
+    <r>
+      <t>size_id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <t>imagen</t>
+  </si>
+  <si>
+    <t>UNIQUE-KEYS</t>
+  </si>
+  <si>
+    <t>SIZES</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>category_id?</t>
+  </si>
+  <si>
+    <r>
+      <t>category_id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <t>CATEGORy</t>
+  </si>
+  <si>
+    <t>GENRES</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <r>
+      <t>category_id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>genre_id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <t>genre_id</t>
+  </si>
+  <si>
+    <t>size_id</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">image_id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">subcategory_id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1785,7 +1858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1881,13 +1954,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1918,6 +1984,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1940,66 +2021,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>60264</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>144623</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>83446</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Flecha: a la izquierda, derecha y arriba 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EB9934DE-6737-4350-9051-6C7E1F2E73F6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="6589734" flipH="1">
-          <a:off x="6993201" y="-878476"/>
-          <a:ext cx="213682" cy="5672562"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftRightUpArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1130299</xdr:colOff>
       <xdr:row>14</xdr:row>
@@ -2016,7 +2037,7 @@
         <xdr:cNvPr id="53" name="Flecha: a la izquierda, derecha y arriba 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2076,7 +2097,7 @@
         <xdr:cNvPr id="54" name="Flecha: a la izquierda, derecha y arriba 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BB06C2DC-CFEB-43E3-ADDB-925B81771409}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB06C2DC-CFEB-43E3-ADDB-925B81771409}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2136,7 +2157,7 @@
         <xdr:cNvPr id="55" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2196,7 +2217,7 @@
         <xdr:cNvPr id="56" name="Flecha: a la izquierda, derecha y arriba 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A357813C-8AF8-4299-BA91-0A528ED1F6BC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A357813C-8AF8-4299-BA91-0A528ED1F6BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2256,7 +2277,7 @@
         <xdr:cNvPr id="57" name="Flecha: a la izquierda, derecha y arriba 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ADF86149-9AF8-4979-9898-D92F280DF2FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADF86149-9AF8-4979-9898-D92F280DF2FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2316,7 +2337,7 @@
         <xdr:cNvPr id="58" name="Flecha: a la izquierda, derecha y arriba 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2A207FFC-329A-4274-9A1D-BEBC97BC4C01}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A207FFC-329A-4274-9A1D-BEBC97BC4C01}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2376,7 +2397,7 @@
         <xdr:cNvPr id="59" name="Flecha: a la izquierda, derecha y arriba 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E1F9FBF-07B9-42FC-AD07-5156F2305EE1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E1F9FBF-07B9-42FC-AD07-5156F2305EE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2436,7 +2457,7 @@
         <xdr:cNvPr id="20" name="Flecha: a la izquierda, derecha y arriba 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2496,7 +2517,7 @@
         <xdr:cNvPr id="22" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2556,7 +2577,7 @@
         <xdr:cNvPr id="23" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2616,7 +2637,7 @@
         <xdr:cNvPr id="24" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2676,7 +2697,7 @@
         <xdr:cNvPr id="17" name="Flecha: a la izquierda, derecha y arriba 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2736,7 +2757,7 @@
         <xdr:cNvPr id="18" name="Flecha: a la izquierda, derecha y arriba 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2A207FFC-329A-4274-9A1D-BEBC97BC4C01}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A207FFC-329A-4274-9A1D-BEBC97BC4C01}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2801,7 +2822,7 @@
         <xdr:cNvPr id="13" name="Conector recto 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2911,7 +2932,7 @@
         <xdr:cNvPr id="2" name="Conector recto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B76CAEE4-09D7-41C5-9067-4444BF67D33E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B76CAEE4-09D7-41C5-9067-4444BF67D33E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2966,7 +2987,7 @@
         <xdr:cNvPr id="16" name="Conector recto 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3016,7 +3037,7 @@
         <xdr:cNvPr id="32" name="Conector recto 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3066,7 +3087,7 @@
         <xdr:cNvPr id="35" name="Conector recto 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3116,7 +3137,7 @@
         <xdr:cNvPr id="36" name="Conector recto 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3166,7 +3187,7 @@
         <xdr:cNvPr id="49" name="Conector recto 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000031000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3216,7 +3237,7 @@
         <xdr:cNvPr id="51" name="Conector recto 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000033000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3266,7 +3287,7 @@
         <xdr:cNvPr id="53" name="Conector recto 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3316,7 +3337,7 @@
         <xdr:cNvPr id="55" name="Conector recto 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000037000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3366,7 +3387,7 @@
         <xdr:cNvPr id="56" name="Conector recto 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3416,7 +3437,7 @@
         <xdr:cNvPr id="59" name="Conector recto 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3466,7 +3487,7 @@
         <xdr:cNvPr id="61" name="Conector recto 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3516,7 +3537,7 @@
         <xdr:cNvPr id="63" name="Conector recto 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3566,7 +3587,7 @@
         <xdr:cNvPr id="66" name="Conector recto 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3616,7 +3637,7 @@
         <xdr:cNvPr id="68" name="Conector recto 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000044000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3666,7 +3687,7 @@
         <xdr:cNvPr id="71" name="Conector recto 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000047000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3716,7 +3737,7 @@
         <xdr:cNvPr id="73" name="Conector recto 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000049000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3766,7 +3787,7 @@
         <xdr:cNvPr id="74" name="Conector recto 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3816,7 +3837,7 @@
         <xdr:cNvPr id="76" name="Conector recto 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3866,7 +3887,7 @@
         <xdr:cNvPr id="81" name="Conector recto 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000051000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3916,7 +3937,7 @@
         <xdr:cNvPr id="82" name="Conector recto 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000052000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3966,7 +3987,7 @@
         <xdr:cNvPr id="86" name="Conector recto 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000056000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4016,7 +4037,7 @@
         <xdr:cNvPr id="87" name="Conector recto 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000057000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4066,7 +4087,7 @@
         <xdr:cNvPr id="90" name="Conector recto 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4116,7 +4137,7 @@
         <xdr:cNvPr id="91" name="Conector recto 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4166,7 +4187,7 @@
         <xdr:cNvPr id="92" name="Conector recto 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4216,7 +4237,7 @@
         <xdr:cNvPr id="93" name="Conector recto 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4266,7 +4287,7 @@
         <xdr:cNvPr id="100" name="Conector recto 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000064000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000064000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4316,7 +4337,7 @@
         <xdr:cNvPr id="101" name="Conector recto 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000065000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4366,7 +4387,7 @@
         <xdr:cNvPr id="106" name="Conector recto 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4416,7 +4437,7 @@
         <xdr:cNvPr id="108" name="Conector recto 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4466,7 +4487,7 @@
         <xdr:cNvPr id="109" name="Conector recto 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4516,7 +4537,7 @@
         <xdr:cNvPr id="111" name="Conector recto 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4566,7 +4587,7 @@
         <xdr:cNvPr id="114" name="Conector recto 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000072000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4616,7 +4637,7 @@
         <xdr:cNvPr id="116" name="Conector recto 115">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000074000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000074000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4666,7 +4687,7 @@
         <xdr:cNvPr id="128" name="Conector recto 127">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000080000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4716,7 +4737,7 @@
         <xdr:cNvPr id="130" name="Conector recto 129">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000082000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4766,7 +4787,7 @@
         <xdr:cNvPr id="131" name="Conector recto 130">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000083000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4816,7 +4837,7 @@
         <xdr:cNvPr id="132" name="Conector recto 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000084000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4866,7 +4887,7 @@
         <xdr:cNvPr id="133" name="Conector recto 132">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000085000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000085000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4916,7 +4937,7 @@
         <xdr:cNvPr id="136" name="Conector recto 135">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000088000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000088000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4966,7 +4987,7 @@
         <xdr:cNvPr id="139" name="Conector recto 138">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5016,7 +5037,7 @@
         <xdr:cNvPr id="141" name="Conector recto 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5066,7 +5087,7 @@
         <xdr:cNvPr id="142" name="Conector recto 141">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5116,7 +5137,7 @@
         <xdr:cNvPr id="143" name="Conector recto 142">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00008F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5440,7 +5461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5450,8 +5471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView topLeftCell="C29" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5485,10 +5506,10 @@
         <v>12</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="R2" s="23"/>
       <c r="S2" s="23"/>
@@ -5496,13 +5517,13 @@
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E3" s="4"/>
       <c r="J3" s="56" t="s">
@@ -5514,10 +5535,10 @@
         <v>1</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5525,10 +5546,10 @@
         <v>18</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E4" s="3"/>
       <c r="J4" s="56" t="s">
@@ -5540,10 +5561,10 @@
         <v>19</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="R4" s="38" t="s">
         <v>23</v>
@@ -5553,10 +5574,10 @@
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="47" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="3"/>
@@ -5581,10 +5602,10 @@
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="47" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="3"/>
@@ -5607,10 +5628,10 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="47" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="3"/>
@@ -5632,13 +5653,13 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="93" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="14"/>
+      <c r="B8" s="124" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="125" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="125"/>
       <c r="E8" s="3"/>
       <c r="J8" s="57" t="s">
         <v>4</v>
@@ -5651,20 +5672,20 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="R8" s="47" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>114</v>
+      <c r="B9" s="126" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="121" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="121" t="s">
+        <v>106</v>
       </c>
       <c r="E9" s="3"/>
       <c r="J9" s="58" t="s">
@@ -5678,20 +5699,20 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="R9" s="47" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>114</v>
+      <c r="B10" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="121" t="s">
+        <v>94</v>
       </c>
       <c r="E10" s="3"/>
       <c r="J10" s="3"/>
@@ -5707,13 +5728,15 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="12"/>
+      <c r="B11" s="127" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="128" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="129" t="s">
+        <v>94</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -5725,22 +5748,18 @@
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="79" t="s">
-        <v>115</v>
-      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="12"/>
       <c r="E12" s="3"/>
       <c r="J12" s="45" t="s">
         <v>8</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -5748,15 +5767,6 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>114</v>
-      </c>
       <c r="E13" s="3"/>
       <c r="J13" s="46" t="s">
         <v>18</v>
@@ -5765,13 +5775,6 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="79" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" s="79"/>
       <c r="E14" s="3"/>
       <c r="J14" s="50" t="s">
         <v>87</v>
@@ -5783,13 +5786,6 @@
       <c r="P14" s="23"/>
     </row>
     <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="80" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="78"/>
       <c r="E15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="47" t="s">
@@ -5800,13 +5796,13 @@
       <c r="M15" s="4"/>
       <c r="P15" s="27"/>
       <c r="R15" s="45" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="T15" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5855,10 +5851,10 @@
         <v>79</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="M19" s="3"/>
       <c r="Q19" s="23"/>
@@ -5893,7 +5889,7 @@
       <c r="E22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -5901,7 +5897,7 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>15</v>
@@ -5917,7 +5913,7 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>0</v>
@@ -5933,7 +5929,7 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B25" s="51" t="s">
         <v>21</v>
@@ -5947,7 +5943,7 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B26" s="45" t="s">
         <v>20</v>
@@ -5963,19 +5959,19 @@
       <c r="E27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="45" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B28" s="51" t="s">
         <v>84</v>
@@ -5985,26 +5981,26 @@
         <v>21</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="46" t="s">
         <v>18</v>
       </c>
       <c r="K28" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>30</v>
@@ -6014,76 +6010,80 @@
         <v>18</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="47" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="K29" s="47" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B30" s="45" t="s">
         <v>22</v>
       </c>
       <c r="F30" s="46" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="47" t="s">
+      <c r="J30" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="L30" s="1"/>
+      <c r="K30" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>79</v>
       </c>
       <c r="F31" s="54" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H31" s="55"/>
-      <c r="J31" s="48" t="s">
+      <c r="J31" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="K31" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="L31" s="2"/>
+      <c r="K31" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B32" s="45" t="s">
         <v>8</v>
@@ -6105,7 +6105,7 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B34" s="51" t="s">
         <v>12</v>
@@ -6114,27 +6114,27 @@
         <v>84</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="45" t="s">
         <v>30</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B35" s="45" t="s">
         <v>19</v>
@@ -6155,7 +6155,7 @@
     </row>
     <row r="36" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B36" s="45" t="s">
         <v>1</v>
@@ -6178,10 +6178,10 @@
     </row>
     <row r="37" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B37" s="84" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>34</v>
@@ -6222,20 +6222,20 @@
         <v>85</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="45" t="s">
         <v>22</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="M41" s="3"/>
     </row>
@@ -6261,7 +6261,7 @@
       <c r="H43" s="12"/>
       <c r="I43" s="3"/>
       <c r="J43" s="47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K43" s="47"/>
       <c r="L43" s="1"/>
@@ -6299,13 +6299,13 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F47" s="45" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
@@ -6314,14 +6314,14 @@
       <c r="M47" s="3"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F48" s="85" t="s">
+      <c r="F48" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>111</v>
+      <c r="G48" s="117" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" s="118" t="s">
+        <v>103</v>
       </c>
       <c r="I48" s="43"/>
       <c r="J48" s="3"/>
@@ -6330,13 +6330,13 @@
       <c r="M48" s="3"/>
     </row>
     <row r="49" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F49" s="86" t="s">
+      <c r="F49" s="119" t="s">
+        <v>133</v>
+      </c>
+      <c r="G49" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="G49" s="92" t="s">
-        <v>124</v>
-      </c>
-      <c r="H49" s="87"/>
+      <c r="H49" s="120"/>
       <c r="I49" s="43"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -6344,13 +6344,13 @@
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F50" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="G50" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="H50" s="89"/>
+      <c r="F50" s="119" t="s">
+        <v>134</v>
+      </c>
+      <c r="G50" s="117" t="s">
+        <v>107</v>
+      </c>
+      <c r="H50" s="120"/>
       <c r="I50" s="43"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -6358,24 +6358,28 @@
       <c r="M50" s="3"/>
     </row>
     <row r="51" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F51" s="86" t="s">
+      <c r="F51" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="G51" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="H51" s="87"/>
+      <c r="G51" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="H51" s="120" t="s">
+        <v>94</v>
+      </c>
       <c r="I51" s="43"/>
       <c r="M51" s="3"/>
     </row>
     <row r="52" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F52" s="90" t="s">
+      <c r="F52" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="G52" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="H52" s="91"/>
+      <c r="G52" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="H52" s="123" t="s">
+        <v>94</v>
+      </c>
       <c r="I52" s="44"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -6437,8 +6441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6461,49 +6465,49 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="23" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="94" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="95" t="s">
-        <v>109</v>
+        <v>119</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>170</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="86" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="93" t="s">
-        <v>134</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="L2" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="M2" s="97" t="s">
-        <v>142</v>
-      </c>
       <c r="N2" s="38" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="O2" s="63" t="s">
         <v>4</v>
@@ -6517,10 +6521,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="65">
@@ -6533,7 +6537,7 @@
         <v>1000</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I3" s="21"/>
       <c r="J3" s="21">
@@ -6550,10 +6554,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="3"/>
@@ -6567,7 +6571,7 @@
         <v>250</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21">
@@ -6584,10 +6588,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="3"/>
@@ -6601,7 +6605,7 @@
         <v>500</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="21">
@@ -6618,10 +6622,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="3"/>
@@ -6635,7 +6639,7 @@
         <v>300</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="21">
@@ -6651,11 +6655,11 @@
       <c r="P6" s="66"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="93" t="s">
-        <v>134</v>
+      <c r="A7" s="86" t="s">
+        <v>123</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="3"/>
@@ -6669,7 +6673,7 @@
         <v>1200</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21">
@@ -6686,13 +6690,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="65">
@@ -6705,7 +6709,7 @@
         <v>600</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21">
@@ -6722,13 +6726,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="65">
@@ -6741,7 +6745,7 @@
         <v>900</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21">
@@ -6758,10 +6762,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="3"/>
@@ -6775,7 +6779,7 @@
         <v>700</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="21">
@@ -6792,10 +6796,10 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="3"/>
@@ -6809,7 +6813,7 @@
         <v>900</v>
       </c>
       <c r="H11" s="68" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I11" s="68"/>
       <c r="J11" s="68">
@@ -6826,13 +6830,13 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -6853,7 +6857,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="79" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C13" s="79"/>
       <c r="D13" s="3"/>
@@ -6875,7 +6879,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="80" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C14" s="78"/>
       <c r="D14" s="3"/>
@@ -6912,13 +6916,13 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
-        <v>8</v>
+        <v>178</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="61" t="s">
@@ -7030,10 +7034,10 @@
         <v>78</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="E22" s="61" t="s">
         <v>18</v>
@@ -7244,7 +7248,7 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="E32" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F32" s="36"/>
       <c r="G32" s="34"/>
@@ -7254,27 +7258,27 @@
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
-        <v>30</v>
+        <v>179</v>
       </c>
       <c r="B33" s="59" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="101" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" s="104" t="s">
-        <v>149</v>
-      </c>
-      <c r="H33" s="102" t="s">
+      <c r="F33" s="95" t="s">
+        <v>180</v>
+      </c>
+      <c r="G33" s="97" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="I33" s="103" t="s">
+      <c r="I33" s="96" t="s">
         <v>3</v>
       </c>
       <c r="J33" s="40"/>
@@ -7286,13 +7290,13 @@
       </c>
       <c r="B34" s="38"/>
       <c r="C34" s="12"/>
-      <c r="E34" s="99">
+      <c r="E34" s="92">
         <v>1</v>
       </c>
       <c r="F34" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="100">
+      <c r="G34" s="93">
         <v>1</v>
       </c>
       <c r="H34" s="37"/>
@@ -7302,7 +7306,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="B35" s="47"/>
       <c r="C35" s="1"/>
@@ -7364,19 +7368,19 @@
         <v>84</v>
       </c>
       <c r="B39" s="60" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C39" s="52" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="E39" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F39" s="62" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="G39" s="62" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="H39" s="63" t="s">
         <v>4</v>
@@ -7405,7 +7409,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="47" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="B41" s="47"/>
       <c r="C41" s="1"/>
@@ -7413,7 +7417,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G41" s="39">
         <v>5</v>
@@ -7423,7 +7427,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="47" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="B42" s="47"/>
       <c r="C42" s="1"/>
@@ -7431,7 +7435,7 @@
         <v>3</v>
       </c>
       <c r="F42" s="68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G42" s="69">
         <v>7</v>
@@ -7458,27 +7462,27 @@
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="E45" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="45" t="s">
-        <v>22</v>
+        <v>174</v>
       </c>
       <c r="B46" s="59" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C46" s="49" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="E46" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F46" s="62" t="s">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="G46" s="62" t="s">
-        <v>103</v>
+        <v>177</v>
       </c>
       <c r="H46" s="63" t="s">
         <v>4</v>
@@ -7507,7 +7511,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="47" t="s">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="B48" s="47"/>
       <c r="C48" s="1"/>
@@ -7525,7 +7529,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="B49" s="53"/>
       <c r="C49" s="42"/>
@@ -7583,28 +7587,28 @@
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="51" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="B53" s="60" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="E53" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F53" s="82" t="s">
-        <v>100</v>
+        <v>171</v>
       </c>
       <c r="G53" s="82" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="H53" s="82" t="s">
         <v>4</v>
       </c>
       <c r="I53" s="82" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -7619,15 +7623,15 @@
       <c r="F54" s="37">
         <v>1</v>
       </c>
-      <c r="G54" s="105">
+      <c r="G54" s="98">
         <v>1</v>
       </c>
-      <c r="H54" s="100"/>
+      <c r="H54" s="93"/>
       <c r="I54" s="77"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="47" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="B55" s="47"/>
       <c r="C55" s="1"/>
@@ -7645,7 +7649,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="B56" s="47"/>
       <c r="C56" s="1"/>
@@ -7663,7 +7667,7 @@
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="53" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="B57" s="53"/>
       <c r="C57" s="42"/>
@@ -7671,7 +7675,7 @@
         <v>4</v>
       </c>
       <c r="F57" s="68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G57" s="69">
         <v>6</v>
@@ -7706,19 +7710,19 @@
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="45" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B61" s="59" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C61" s="49" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="E61" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F61" s="63" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="G61" s="63" t="s">
         <v>4</v>
@@ -7732,10 +7736,10 @@
         <v>18</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E62" s="65">
         <v>1</v>
@@ -7748,10 +7752,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="B63" s="96" t="s">
         <v>129</v>
+      </c>
+      <c r="B63" s="89" t="s">
+        <v>118</v>
       </c>
       <c r="C63" s="1"/>
       <c r="E63" s="65">
@@ -7768,14 +7772,14 @@
         <v>4</v>
       </c>
       <c r="B64" s="79" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C64" s="1"/>
       <c r="E64" s="65">
         <v>3</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G64" s="21"/>
       <c r="H64" s="66"/>
@@ -7785,7 +7789,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="79" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C65" s="2"/>
       <c r="E65" s="67">
@@ -7808,22 +7812,22 @@
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B67" s="59" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C67" s="49" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="E67" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F67" s="62" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G67" s="62" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="H67" s="63" t="s">
         <v>4</v>
@@ -7837,16 +7841,16 @@
         <v>18</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E68" s="65">
         <v>1</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G68" s="39">
         <v>20</v>
@@ -7856,17 +7860,17 @@
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="85" t="s">
         <v>144</v>
-      </c>
-      <c r="B69" s="92" t="s">
-        <v>124</v>
       </c>
       <c r="C69" s="1"/>
       <c r="E69" s="65">
         <v>2</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G69" s="39">
         <v>18</v>
@@ -7875,18 +7879,18 @@
       <c r="I69" s="66"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="98" t="s">
-        <v>145</v>
+      <c r="A70" s="91" t="s">
+        <v>134</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C70" s="42"/>
       <c r="E70" s="65">
         <v>3</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G70" s="39">
         <v>23</v>
@@ -7899,14 +7903,14 @@
         <v>4</v>
       </c>
       <c r="B71" s="79" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C71" s="1"/>
       <c r="E71" s="67">
         <v>4</v>
       </c>
       <c r="F71" s="68" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G71" s="69">
         <v>1</v>
@@ -7919,7 +7923,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="79" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C72" s="2"/>
       <c r="E72" s="3"/>
@@ -7930,22 +7934,22 @@
     <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="51" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B74" s="60" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C74" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="E74" s="101" t="s">
+        <v>159</v>
+      </c>
+      <c r="E74" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="F74" s="106" t="s">
-        <v>146</v>
-      </c>
-      <c r="G74" s="106" t="s">
-        <v>147</v>
+      <c r="F74" s="99" t="s">
+        <v>135</v>
+      </c>
+      <c r="G74" s="99" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -7953,12 +7957,12 @@
         <v>18</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E75" s="99">
+        <v>103</v>
+      </c>
+      <c r="E75" s="92">
         <v>1</v>
       </c>
       <c r="F75" s="37">
@@ -7970,10 +7974,10 @@
     </row>
     <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="46" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C76" s="12"/>
       <c r="E76" s="65">
@@ -7988,10 +7992,10 @@
     </row>
     <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="54" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C77" s="55"/>
       <c r="E77" s="67">
@@ -8007,21 +8011,21 @@
     <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="45" t="s">
-        <v>19</v>
+        <v>166</v>
       </c>
       <c r="B79" s="59" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C79" s="49" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E79" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F79" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="G79" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="G79" s="115" t="s">
         <v>7</v>
       </c>
       <c r="H79" s="64" t="s">
@@ -8036,10 +8040,10 @@
         <v>23</v>
       </c>
       <c r="B80" s="38" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E80" s="65">
         <v>1</v>
@@ -8048,7 +8052,7 @@
         <v>28</v>
       </c>
       <c r="G80" s="31" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H80" s="31"/>
       <c r="I80" s="66"/>
@@ -8056,20 +8060,20 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="38" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B81" s="38" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E81" s="65">
         <v>2</v>
       </c>
       <c r="F81" s="21"/>
       <c r="G81" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="H81" s="31"/>
       <c r="I81" s="66"/>
@@ -8093,7 +8097,7 @@
         <v>4</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C83" s="1"/>
       <c r="E83" s="65"/>
@@ -8107,7 +8111,7 @@
         <v>3</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C84" s="2"/>
       <c r="E84" s="67"/>
@@ -8119,27 +8123,27 @@
     <row r="85" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="51" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B86" s="60" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C86" s="52" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E86" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F86" s="72" t="s">
-        <v>35</v>
+        <v>167</v>
       </c>
       <c r="G86" s="72" t="s">
-        <v>147</v>
-      </c>
-      <c r="H86" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="H86" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="I86" s="108" t="s">
+      <c r="I86" s="101" t="s">
         <v>14</v>
       </c>
     </row>
@@ -8148,13 +8152,13 @@
         <v>18</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="D87" s="107" t="s">
-        <v>151</v>
+        <v>155</v>
+      </c>
+      <c r="D87" s="100" t="s">
+        <v>139</v>
       </c>
       <c r="E87" s="65">
         <v>1</v>
@@ -8165,10 +8169,10 @@
       <c r="G87" s="21">
         <v>7</v>
       </c>
-      <c r="H87" s="109" t="s">
-        <v>154</v>
-      </c>
-      <c r="I87" s="109"/>
+      <c r="H87" s="102" t="s">
+        <v>142</v>
+      </c>
+      <c r="I87" s="102"/>
       <c r="J87" s="63" t="s">
         <v>3</v>
       </c>
@@ -8181,70 +8185,70 @@
         <v>35</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E88" s="65">
         <v>2</v>
       </c>
       <c r="F88" s="21"/>
       <c r="G88" s="21"/>
-      <c r="H88" s="109"/>
-      <c r="I88" s="109"/>
+      <c r="H88" s="102"/>
+      <c r="I88" s="102"/>
       <c r="J88" s="21"/>
       <c r="K88" s="66"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="56" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E89" s="65">
         <v>3</v>
       </c>
       <c r="F89" s="21"/>
       <c r="G89" s="21"/>
-      <c r="H89" s="109"/>
-      <c r="I89" s="109"/>
+      <c r="H89" s="102"/>
+      <c r="I89" s="102"/>
       <c r="J89" s="21"/>
       <c r="K89" s="66"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="111" t="s">
-        <v>13</v>
-      </c>
-      <c r="B90" s="112"/>
-      <c r="C90" s="113"/>
+      <c r="A90" s="104" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="105"/>
+      <c r="C90" s="106"/>
       <c r="E90" s="65">
         <v>4</v>
       </c>
       <c r="F90" s="21"/>
       <c r="G90" s="21"/>
-      <c r="H90" s="109"/>
-      <c r="I90" s="109"/>
+      <c r="H90" s="102"/>
+      <c r="I90" s="102"/>
       <c r="J90" s="21"/>
       <c r="K90" s="66"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="111" t="s">
+      <c r="A91" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="B91" s="112"/>
-      <c r="C91" s="113"/>
+      <c r="B91" s="105"/>
+      <c r="C91" s="106"/>
       <c r="E91" s="65">
         <v>5</v>
       </c>
       <c r="F91" s="21"/>
       <c r="G91" s="21"/>
-      <c r="H91" s="109"/>
-      <c r="I91" s="109"/>
+      <c r="H91" s="102"/>
+      <c r="I91" s="102"/>
       <c r="J91" s="21"/>
       <c r="K91" s="66"/>
     </row>
@@ -8253,7 +8257,7 @@
         <v>4</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C92" s="1"/>
       <c r="E92" s="65">
@@ -8261,8 +8265,8 @@
       </c>
       <c r="F92" s="21"/>
       <c r="G92" s="21"/>
-      <c r="H92" s="109"/>
-      <c r="I92" s="109"/>
+      <c r="H92" s="102"/>
+      <c r="I92" s="102"/>
       <c r="J92" s="21"/>
       <c r="K92" s="66"/>
     </row>
@@ -8271,7 +8275,7 @@
         <v>3</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C93" s="2"/>
       <c r="E93" s="67">
@@ -8279,44 +8283,44 @@
       </c>
       <c r="F93" s="68"/>
       <c r="G93" s="68"/>
-      <c r="H93" s="110"/>
-      <c r="I93" s="110"/>
+      <c r="H93" s="103"/>
+      <c r="I93" s="103"/>
       <c r="J93" s="21"/>
       <c r="K93" s="66"/>
     </row>
     <row r="94" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E94" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="J94" s="117"/>
+        <v>143</v>
+      </c>
+      <c r="J94" s="110"/>
       <c r="K94" s="71"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="94" t="s">
-        <v>169</v>
-      </c>
-      <c r="B95" s="94" t="s">
-        <v>170</v>
-      </c>
-      <c r="C95" s="95" t="s">
-        <v>171</v>
-      </c>
-      <c r="E95" s="119" t="s">
+      <c r="A95" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="87" t="s">
+        <v>158</v>
+      </c>
+      <c r="C95" s="88" t="s">
+        <v>159</v>
+      </c>
+      <c r="E95" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="F95" s="119" t="s">
-        <v>131</v>
-      </c>
-      <c r="G95" s="119" t="s">
+      <c r="F95" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="G95" s="112" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="63" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="I95" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="J95" s="114" t="s">
+      <c r="J95" s="107" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8325,47 +8329,47 @@
         <v>23</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E96" s="65">
         <v>23</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="G96" s="120" t="s">
-        <v>162</v>
+        <v>146</v>
+      </c>
+      <c r="G96" s="113" t="s">
+        <v>150</v>
       </c>
       <c r="H96" s="21">
         <v>123456</v>
       </c>
-      <c r="I96" s="115"/>
+      <c r="I96" s="108"/>
       <c r="J96" s="21"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C97" s="21"/>
       <c r="E97" s="65">
         <v>33</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="G97" s="120" t="s">
-        <v>163</v>
+        <v>145</v>
+      </c>
+      <c r="G97" s="113" t="s">
+        <v>151</v>
       </c>
       <c r="H97" s="21">
         <v>853697</v>
       </c>
-      <c r="I97" s="115"/>
+      <c r="I97" s="108"/>
       <c r="J97" s="21"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -8373,83 +8377,93 @@
         <v>5</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C98" s="21"/>
+        <v>144</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>173</v>
+      </c>
       <c r="E98" s="65">
         <v>58</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="G98" s="120" t="s">
-        <v>164</v>
+        <v>147</v>
+      </c>
+      <c r="G98" s="113" t="s">
+        <v>152</v>
       </c>
       <c r="H98" s="21">
         <v>421586</v>
       </c>
-      <c r="I98" s="115"/>
+      <c r="I98" s="108"/>
       <c r="J98" s="21"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C99" s="21"/>
       <c r="E99" s="65">
         <v>102</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="G99" s="120" t="s">
-        <v>166</v>
+        <v>148</v>
+      </c>
+      <c r="G99" s="113" t="s">
+        <v>154</v>
       </c>
       <c r="H99" s="21">
         <v>754896</v>
       </c>
-      <c r="I99" s="115"/>
+      <c r="I99" s="108"/>
       <c r="J99" s="21"/>
     </row>
     <row r="100" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B100" s="20" t="s">
-        <v>153</v>
+      <c r="A100" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" s="34" t="s">
+        <v>144</v>
       </c>
       <c r="C100" s="21"/>
       <c r="E100" s="67">
         <v>200</v>
       </c>
       <c r="F100" s="68" t="s">
-        <v>161</v>
-      </c>
-      <c r="G100" s="121" t="s">
-        <v>165</v>
+        <v>149</v>
+      </c>
+      <c r="G100" s="114" t="s">
+        <v>153</v>
       </c>
       <c r="H100" s="68">
         <v>214659</v>
       </c>
-      <c r="I100" s="116"/>
+      <c r="I100" s="109"/>
       <c r="J100" s="21"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C101" s="21"/>
       <c r="J101" s="3"/>
     </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
@@ -8471,7 +8485,7 @@
       <c r="M106" s="3"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I107" s="118"/>
+      <c r="I107" s="111"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>

</xml_diff>

<commit_message>
base de datos User
</commit_message>
<xml_diff>
--- a/tablas_ base de datos.xlsx
+++ b/tablas_ base de datos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr checkCompatibility="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BASE DE DATOS" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="198">
   <si>
     <t>PRODUCTOS</t>
   </si>
@@ -668,15 +668,6 @@
     <t>DATETIME</t>
   </si>
   <si>
-    <t>imagenUsuario</t>
-  </si>
-  <si>
-    <t>categoriaUsuario-id</t>
-  </si>
-  <si>
-    <t>CATEGORIAUSUARIOS</t>
-  </si>
-  <si>
     <t>flor</t>
   </si>
   <si>
@@ -934,9 +925,6 @@
     <t>*A</t>
   </si>
   <si>
-    <t>*A puede tener 2 restricciones ej.Auto increment y UNIQUE KEYS?</t>
-  </si>
-  <si>
     <t>TIMESTAMP</t>
   </si>
   <si>
@@ -1086,9 +1074,6 @@
     <t>imagen</t>
   </si>
   <si>
-    <t>UNIQUE-KEYS</t>
-  </si>
-  <si>
     <t>SIZES</t>
   </si>
   <si>
@@ -1205,12 +1190,96 @@
       <t>(FK)</t>
     </r>
   </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>safePrice</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <r>
+      <t>userType</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>AUTO-INCRMENT/NOT NULL</t>
+  </si>
+  <si>
+    <t>userTypeS</t>
+  </si>
+  <si>
+    <t>userTypes</t>
+  </si>
+  <si>
+    <t>created-at</t>
+  </si>
+  <si>
+    <t>updated_ut</t>
+  </si>
+  <si>
+    <r>
+      <t>userType_id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(FK)</t>
+    </r>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>Admi</t>
+  </si>
+  <si>
+    <r>
+      <t>VARCHAR(255</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1279,6 +1348,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1858,7 +1942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1999,6 +2083,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2856,16 +2949,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2889,7 +2982,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="20459700"/>
+          <a:off x="5915025" y="22031325"/>
           <a:ext cx="7286625" cy="1571625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5471,8 +5564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30:K31"/>
+    <sheetView topLeftCell="L2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5495,7 +5588,7 @@
     <col min="16" max="16" width="15.7109375" customWidth="1"/>
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
     <col min="18" max="18" width="33" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
     <col min="20" max="20" width="18.140625" customWidth="1"/>
     <col min="22" max="22" width="33" bestFit="1" customWidth="1"/>
   </cols>
@@ -5515,9 +5608,9 @@
       <c r="S2" s="23"/>
       <c r="T2" s="23"/>
     </row>
-    <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>100</v>
@@ -5531,17 +5624,17 @@
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="R3" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="S3" s="132" t="s">
+        <v>154</v>
+      </c>
+      <c r="T3" s="132" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="73" t="s">
         <v>18</v>
       </c>
@@ -5566,15 +5659,15 @@
       <c r="P4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="R4" s="38" t="s">
+      <c r="R4" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S4" s="134"/>
+      <c r="T4" s="134"/>
+    </row>
+    <row r="5" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="47" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>104</v>
@@ -5594,15 +5687,15 @@
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
-      <c r="R5" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="R5" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="S5" s="134"/>
+      <c r="T5" s="134"/>
+    </row>
+    <row r="6" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="47" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>105</v>
@@ -5620,15 +5713,15 @@
       </c>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
-      <c r="R6" s="47" t="s">
+      <c r="R6" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S6" s="136"/>
+      <c r="T6" s="136"/>
+    </row>
+    <row r="7" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="47" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>104</v>
@@ -5646,15 +5739,15 @@
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="R7" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="R7" s="135" t="s">
+        <v>156</v>
+      </c>
+      <c r="S7" s="136"/>
+      <c r="T7" s="136"/>
+    </row>
+    <row r="8" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="124" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C8" s="125" t="s">
         <v>107</v>
@@ -5671,15 +5764,15 @@
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="R8" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R8" s="135" t="s">
+        <v>130</v>
+      </c>
+      <c r="S8" s="136"/>
+      <c r="T8" s="136"/>
+    </row>
+    <row r="9" spans="2:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="126" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C9" s="121" t="s">
         <v>107</v>
@@ -5698,18 +5791,18 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="R9" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="R9" s="135" t="s">
+        <v>186</v>
+      </c>
+      <c r="S9" s="136"/>
+      <c r="T9" s="136"/>
+    </row>
+    <row r="10" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="91" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="121" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D10" s="121" t="s">
         <v>94</v>
@@ -5721,18 +5814,18 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="R10" s="47" t="s">
+      <c r="R10" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S10" s="136"/>
+      <c r="T10" s="136"/>
+    </row>
+    <row r="11" spans="2:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="127" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="128" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D11" s="129" t="s">
         <v>94</v>
@@ -5741,11 +5834,11 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="R11" s="48" t="s">
+      <c r="R11" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
+      <c r="S11" s="138"/>
+      <c r="T11" s="138"/>
     </row>
     <row r="12" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="38"/>
@@ -5796,13 +5889,13 @@
       <c r="M15" s="4"/>
       <c r="P15" s="27"/>
       <c r="R15" s="45" t="s">
-        <v>111</v>
+        <v>189</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="T15" s="10" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5826,7 +5919,7 @@
       <c r="I17" s="3"/>
       <c r="M17" s="3"/>
       <c r="R17" s="38" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
@@ -5897,7 +5990,7 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>15</v>
@@ -5913,7 +6006,7 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>0</v>
@@ -5929,7 +6022,7 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B25" s="51" t="s">
         <v>21</v>
@@ -5943,7 +6036,7 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B26" s="45" t="s">
         <v>20</v>
@@ -5959,7 +6052,7 @@
       <c r="E27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="45" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K27" s="10" t="s">
         <v>100</v>
@@ -5971,7 +6064,7 @@
     </row>
     <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B28" s="51" t="s">
         <v>84</v>
@@ -6000,7 +6093,7 @@
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>30</v>
@@ -6017,7 +6110,7 @@
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="47" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K29" s="47" t="s">
         <v>104</v>
@@ -6030,13 +6123,13 @@
     </row>
     <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B30" s="45" t="s">
         <v>22</v>
       </c>
       <c r="F30" s="46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>107</v>
@@ -6047,7 +6140,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="121" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>94</v>
@@ -6057,13 +6150,13 @@
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>79</v>
       </c>
       <c r="F31" s="54" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G31" s="32" t="s">
         <v>107</v>
@@ -6073,7 +6166,7 @@
         <v>3</v>
       </c>
       <c r="K31" s="121" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>94</v>
@@ -6083,7 +6176,7 @@
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B32" s="45" t="s">
         <v>8</v>
@@ -6105,7 +6198,7 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B34" s="51" t="s">
         <v>12</v>
@@ -6134,7 +6227,7 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B35" s="45" t="s">
         <v>19</v>
@@ -6155,7 +6248,7 @@
     </row>
     <row r="36" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B36" s="45" t="s">
         <v>1</v>
@@ -6178,10 +6271,10 @@
     </row>
     <row r="37" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B37" s="84" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>34</v>
@@ -6299,7 +6392,7 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F47" s="45" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>100</v>
@@ -6331,10 +6424,10 @@
     </row>
     <row r="49" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F49" s="119" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G49" s="89" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H49" s="120"/>
       <c r="I49" s="43"/>
@@ -6345,7 +6438,7 @@
     </row>
     <row r="50" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F50" s="119" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G50" s="117" t="s">
         <v>107</v>
@@ -6362,7 +6455,7 @@
         <v>4</v>
       </c>
       <c r="G51" s="121" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H51" s="120" t="s">
         <v>94</v>
@@ -6375,7 +6468,7 @@
         <v>3</v>
       </c>
       <c r="G52" s="121" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H52" s="123" t="s">
         <v>94</v>
@@ -6439,10 +6532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:N11"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6465,49 +6558,49 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B2" s="87" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="88" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="J2" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="K2" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="I2" s="86" t="s">
+      <c r="L2" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="M2" s="90" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" s="38" t="s">
         <v>124</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="M2" s="90" t="s">
-        <v>131</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>127</v>
       </c>
       <c r="O2" s="63" t="s">
         <v>4</v>
@@ -6554,7 +6647,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>104</v>
@@ -6588,7 +6681,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>105</v>
@@ -6622,7 +6715,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>104</v>
@@ -6656,7 +6749,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="86" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B7" s="81" t="s">
         <v>107</v>
@@ -6690,7 +6783,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8" s="79" t="s">
         <v>107</v>
@@ -6726,7 +6819,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B9" s="79" t="s">
         <v>107</v>
@@ -6762,7 +6855,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B10" s="79" t="s">
         <v>107</v>
@@ -6796,7 +6889,7 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B11" s="79" t="s">
         <v>107</v>
@@ -6830,7 +6923,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B12" s="79" t="s">
         <v>107</v>
@@ -6916,13 +7009,13 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="61" t="s">
@@ -7034,10 +7127,10 @@
         <v>78</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E22" s="61" t="s">
         <v>18</v>
@@ -7258,22 +7351,22 @@
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B33" s="59" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E33" s="94" t="s">
         <v>18</v>
       </c>
       <c r="F33" s="95" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G33" s="97" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H33" s="95" t="s">
         <v>4</v>
@@ -7306,7 +7399,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B35" s="47"/>
       <c r="C35" s="1"/>
@@ -7368,19 +7461,19 @@
         <v>84</v>
       </c>
       <c r="B39" s="60" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C39" s="52" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E39" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F39" s="62" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G39" s="62" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H39" s="63" t="s">
         <v>4</v>
@@ -7409,7 +7502,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="47" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B41" s="47"/>
       <c r="C41" s="1"/>
@@ -7427,7 +7520,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B42" s="47"/>
       <c r="C42" s="1"/>
@@ -7467,22 +7560,22 @@
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="45" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B46" s="59" t="s">
         <v>100</v>
       </c>
       <c r="C46" s="49" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E46" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F46" s="62" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G46" s="62" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H46" s="63" t="s">
         <v>4</v>
@@ -7511,7 +7604,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="47" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B48" s="47"/>
       <c r="C48" s="1"/>
@@ -7529,7 +7622,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B49" s="53"/>
       <c r="C49" s="42"/>
@@ -7587,22 +7680,22 @@
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="51" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B53" s="60" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E53" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F53" s="82" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G53" s="82" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H53" s="82" t="s">
         <v>4</v>
@@ -7631,7 +7724,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="47" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B55" s="47"/>
       <c r="C55" s="1"/>
@@ -7649,7 +7742,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B56" s="47"/>
       <c r="C56" s="1"/>
@@ -7667,7 +7760,7 @@
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="53" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B57" s="53"/>
       <c r="C57" s="42"/>
@@ -7710,19 +7803,19 @@
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="45" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B61" s="59" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C61" s="49" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E61" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F61" s="63" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G61" s="63" t="s">
         <v>4</v>
@@ -7752,10 +7845,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B63" s="89" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C63" s="1"/>
       <c r="E63" s="65">
@@ -7772,14 +7865,14 @@
         <v>4</v>
       </c>
       <c r="B64" s="79" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C64" s="1"/>
       <c r="E64" s="65">
         <v>3</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G64" s="21"/>
       <c r="H64" s="66"/>
@@ -7789,7 +7882,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="79" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C65" s="2"/>
       <c r="E65" s="67">
@@ -7812,22 +7905,22 @@
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B67" s="59" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C67" s="49" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E67" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F67" s="62" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G67" s="62" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H67" s="63" t="s">
         <v>4</v>
@@ -7860,10 +7953,10 @@
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B69" s="85" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C69" s="1"/>
       <c r="E69" s="65">
@@ -7880,7 +7973,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="91" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B70" s="32" t="s">
         <v>107</v>
@@ -7903,7 +7996,7 @@
         <v>4</v>
       </c>
       <c r="B71" s="79" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C71" s="1"/>
       <c r="E71" s="67">
@@ -7923,7 +8016,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="79" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C72" s="2"/>
       <c r="E72" s="3"/>
@@ -7934,22 +8027,22 @@
     <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B74" s="60" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C74" s="52" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E74" s="94" t="s">
         <v>18</v>
       </c>
       <c r="F74" s="99" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G74" s="99" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -7974,7 +8067,7 @@
     </row>
     <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B76" s="12" t="s">
         <v>107</v>
@@ -7992,7 +8085,7 @@
     </row>
     <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="54" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B77" s="32" t="s">
         <v>107</v>
@@ -8011,22 +8104,22 @@
     <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="45" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B79" s="59" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C79" s="49" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E79" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F79" s="32" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G79" s="115" t="s">
-        <v>7</v>
+        <v>183</v>
       </c>
       <c r="H79" s="64" t="s">
         <v>4</v>
@@ -8043,7 +8136,7 @@
         <v>107</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E80" s="65">
         <v>1</v>
@@ -8052,35 +8145,35 @@
         <v>28</v>
       </c>
       <c r="G80" s="31" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H80" s="31"/>
       <c r="I80" s="66"/>
       <c r="J80" s="83"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="38" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B81" s="38" t="s">
         <v>107</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E81" s="65">
         <v>2</v>
       </c>
       <c r="F81" s="21"/>
       <c r="G81" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H81" s="31"/>
       <c r="I81" s="66"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="47" t="s">
-        <v>7</v>
+        <v>183</v>
       </c>
       <c r="B82" s="47"/>
       <c r="C82" s="1"/>
@@ -8092,12 +8185,12 @@
       <c r="H82" s="31"/>
       <c r="I82" s="66"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C83" s="1"/>
       <c r="E83" s="65"/>
@@ -8106,12 +8199,12 @@
       <c r="H83" s="31"/>
       <c r="I83" s="66"/>
     </row>
-    <row r="84" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="48" t="s">
         <v>3</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C84" s="2"/>
       <c r="E84" s="67"/>
@@ -8120,25 +8213,25 @@
       <c r="H84" s="70"/>
       <c r="I84" s="71"/>
     </row>
-    <row r="85" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="51" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B86" s="60" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C86" s="52" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E86" s="61" t="s">
         <v>18</v>
       </c>
       <c r="F86" s="72" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G86" s="72" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H86" s="101" t="s">
         <v>13</v>
@@ -8147,7 +8240,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="56" t="s">
         <v>18</v>
       </c>
@@ -8155,10 +8248,10 @@
         <v>107</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D87" s="100" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E87" s="65">
         <v>1</v>
@@ -8170,7 +8263,7 @@
         <v>7</v>
       </c>
       <c r="H87" s="102" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I87" s="102"/>
       <c r="J87" s="63" t="s">
@@ -8180,7 +8273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="56" t="s">
         <v>35</v>
       </c>
@@ -8188,7 +8281,7 @@
         <v>107</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E88" s="65">
         <v>2</v>
@@ -8200,15 +8293,15 @@
       <c r="J88" s="21"/>
       <c r="K88" s="66"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="56" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B89" s="38" t="s">
         <v>107</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E89" s="65">
         <v>3</v>
@@ -8220,9 +8313,9 @@
       <c r="J89" s="21"/>
       <c r="K89" s="66"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="104" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B90" s="105"/>
       <c r="C90" s="106"/>
@@ -8236,9 +8329,9 @@
       <c r="J90" s="21"/>
       <c r="K90" s="66"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="104" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="B91" s="105"/>
       <c r="C91" s="106"/>
@@ -8252,12 +8345,12 @@
       <c r="J91" s="21"/>
       <c r="K91" s="66"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="57" t="s">
         <v>4</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C92" s="1"/>
       <c r="E92" s="65">
@@ -8270,12 +8363,12 @@
       <c r="J92" s="21"/>
       <c r="K92" s="66"/>
     </row>
-    <row r="93" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="58" t="s">
         <v>3</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C93" s="2"/>
       <c r="E93" s="67">
@@ -8288,43 +8381,49 @@
       <c r="J93" s="21"/>
       <c r="K93" s="66"/>
     </row>
-    <row r="94" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E94" s="23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J94" s="110"/>
       <c r="K94" s="71"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="87" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B95" s="87" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C95" s="88" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E95" s="112" t="s">
         <v>23</v>
       </c>
       <c r="F95" s="112" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G95" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="H95" s="63" t="s">
-        <v>160</v>
-      </c>
-      <c r="I95" s="63" t="s">
+      <c r="H95" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I95" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="J95" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="K95" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="J95" s="107" t="s">
+      <c r="L95" s="107" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="20" t="s">
         <v>23</v>
       </c>
@@ -8332,138 +8431,176 @@
         <v>107</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E96" s="65">
         <v>23</v>
       </c>
       <c r="F96" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G96" s="113" t="s">
         <v>146</v>
-      </c>
-      <c r="G96" s="113" t="s">
-        <v>150</v>
       </c>
       <c r="H96" s="21">
         <v>123456</v>
       </c>
-      <c r="I96" s="108"/>
-      <c r="J96" s="21"/>
+      <c r="I96" s="21">
+        <v>1</v>
+      </c>
+      <c r="J96" s="21">
+        <v>0</v>
+      </c>
+      <c r="K96" s="108"/>
+      <c r="L96" s="21"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C97" s="21"/>
       <c r="E97" s="65">
         <v>33</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G97" s="113" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H97" s="21">
         <v>853697</v>
       </c>
-      <c r="I97" s="108"/>
-      <c r="J97" s="21"/>
+      <c r="I97" s="21">
+        <v>8</v>
+      </c>
+      <c r="J97" s="21">
+        <v>0</v>
+      </c>
+      <c r="K97" s="108"/>
+      <c r="L97" s="21"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C98" s="21" t="s">
-        <v>173</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C98" s="21"/>
       <c r="E98" s="65">
         <v>58</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G98" s="113" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H98" s="21">
         <v>421586</v>
       </c>
-      <c r="I98" s="108"/>
-      <c r="J98" s="21"/>
+      <c r="I98" s="21">
+        <v>2</v>
+      </c>
+      <c r="J98" s="21">
+        <v>1</v>
+      </c>
+      <c r="K98" s="108"/>
+      <c r="L98" s="21"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C99" s="21"/>
       <c r="E99" s="65">
         <v>102</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G99" s="113" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H99" s="21">
         <v>754896</v>
       </c>
-      <c r="I99" s="108"/>
-      <c r="J99" s="21"/>
+      <c r="I99" s="21">
+        <v>1</v>
+      </c>
+      <c r="J99" s="21">
+        <v>1</v>
+      </c>
+      <c r="K99" s="108"/>
+      <c r="L99" s="21"/>
     </row>
     <row r="100" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="36" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B100" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="C100" s="21"/>
+        <v>197</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="E100" s="67">
         <v>200</v>
       </c>
       <c r="F100" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="G100" s="114" t="s">
         <v>149</v>
       </c>
-      <c r="G100" s="114" t="s">
-        <v>153</v>
-      </c>
-      <c r="H100" s="68">
+      <c r="H100" s="21">
         <v>214659</v>
       </c>
-      <c r="I100" s="109"/>
-      <c r="J100" s="21"/>
+      <c r="I100" s="21">
+        <v>8</v>
+      </c>
+      <c r="J100" s="21">
+        <v>0</v>
+      </c>
+      <c r="K100" s="109"/>
+      <c r="L100" s="21"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A101" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B101" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="C101" s="21"/>
+      <c r="A101" t="s">
+        <v>193</v>
+      </c>
+      <c r="B101" s="34" t="s">
+        <v>195</v>
+      </c>
       <c r="J101" s="3"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C102" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>140</v>
+      <c r="B103" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
@@ -8472,19 +8609,59 @@
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
       <c r="M105" s="3"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E106" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="F106" s="112" t="s">
+        <v>187</v>
+      </c>
+      <c r="G106" s="112" t="s">
+        <v>191</v>
+      </c>
+      <c r="H106" s="63" t="s">
+        <v>192</v>
+      </c>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
       <c r="M106" s="3"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E107" s="65">
+        <v>0</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="G107" s="113"/>
+      <c r="H107" s="21">
+        <v>123456</v>
+      </c>
       <c r="I107" s="111"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
@@ -8492,6 +8669,23 @@
       <c r="M107" s="3"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" s="130" t="s">
+        <v>187</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C108" s="9"/>
+      <c r="E108" s="65">
+        <v>1</v>
+      </c>
+      <c r="F108" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="G108" s="113"/>
+      <c r="H108" s="21">
+        <v>853697</v>
+      </c>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
@@ -8506,32 +8700,14 @@
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J110" s="3"/>
       <c r="K110" s="3"/>
-      <c r="L110" s="3"/>
-      <c r="M110" s="3"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
-      <c r="L112" s="3"/>
-      <c r="M112" s="3"/>
-    </row>
-    <row r="113" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-    </row>
-    <row r="114" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
-    </row>
-    <row r="115" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J115" s="3"/>
-      <c r="K115" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
con Subcategoria en vista de administrador, usuario y create
</commit_message>
<xml_diff>
--- a/tablas_ base de datos.xlsx
+++ b/tablas_ base de datos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr checkCompatibility="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\carpetaLaura\TP\VisteteDePoder\VisteteDePoder\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EA48C9-C764-48B6-96EE-CDB38D3D606C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE DE DATOS" sheetId="3" r:id="rId1"/>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="197">
   <si>
     <t>PRODUCTOS</t>
   </si>
@@ -1156,27 +1162,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">image_id </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(FK)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">subcategory_id </t>
     </r>
     <r>
@@ -1278,7 +1263,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1408,7 +1393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1851,32 +1836,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1942,7 +1901,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2040,8 +1999,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2051,7 +2010,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2060,24 +2019,17 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2130,7 +2082,7 @@
         <xdr:cNvPr id="53" name="Flecha: a la izquierda, derecha y arriba 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2190,7 +2142,7 @@
         <xdr:cNvPr id="54" name="Flecha: a la izquierda, derecha y arriba 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB06C2DC-CFEB-43E3-ADDB-925B81771409}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2250,7 +2202,7 @@
         <xdr:cNvPr id="55" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2310,7 +2262,7 @@
         <xdr:cNvPr id="56" name="Flecha: a la izquierda, derecha y arriba 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A357813C-8AF8-4299-BA91-0A528ED1F6BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2370,7 +2322,7 @@
         <xdr:cNvPr id="57" name="Flecha: a la izquierda, derecha y arriba 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADF86149-9AF8-4979-9898-D92F280DF2FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,7 +2382,7 @@
         <xdr:cNvPr id="58" name="Flecha: a la izquierda, derecha y arriba 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A207FFC-329A-4274-9A1D-BEBC97BC4C01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2490,7 +2442,7 @@
         <xdr:cNvPr id="59" name="Flecha: a la izquierda, derecha y arriba 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E1F9FBF-07B9-42FC-AD07-5156F2305EE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2550,7 +2502,7 @@
         <xdr:cNvPr id="20" name="Flecha: a la izquierda, derecha y arriba 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2610,7 +2562,7 @@
         <xdr:cNvPr id="22" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2670,7 +2622,7 @@
         <xdr:cNvPr id="23" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2730,7 +2682,7 @@
         <xdr:cNvPr id="24" name="Flecha: a la izquierda, derecha y arriba 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54FE6F7-3D15-4ACE-B6E3-A1D7020CBE57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2790,7 +2742,7 @@
         <xdr:cNvPr id="17" name="Flecha: a la izquierda, derecha y arriba 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3097E1F8-85AD-4C9B-A988-60B813646FDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2800,66 +2752,6 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="24904698" y="2222500"/>
           <a:ext cx="215901" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftRightUpArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>526384</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>109202</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>784546</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>97912</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Flecha: a la izquierda, derecha y arriba 57">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A207FFC-329A-4274-9A1D-BEBC97BC4C01}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="20516351">
-          <a:off x="4310984" y="2877802"/>
-          <a:ext cx="258162" cy="6986410"/>
         </a:xfrm>
         <a:prstGeom prst="leftRightUpArrow">
           <a:avLst/>
@@ -2915,7 +2807,7 @@
         <xdr:cNvPr id="13" name="Conector recto 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2962,7 +2854,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="4 Imagen"/>
+        <xdr:cNvPr id="5" name="4 Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3025,7 +2923,7 @@
         <xdr:cNvPr id="2" name="Conector recto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B76CAEE4-09D7-41C5-9067-4444BF67D33E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3080,7 +2978,7 @@
         <xdr:cNvPr id="16" name="Conector recto 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3130,7 +3028,7 @@
         <xdr:cNvPr id="32" name="Conector recto 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3180,7 +3078,7 @@
         <xdr:cNvPr id="35" name="Conector recto 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3230,7 +3128,7 @@
         <xdr:cNvPr id="36" name="Conector recto 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3280,7 +3178,7 @@
         <xdr:cNvPr id="49" name="Conector recto 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3330,7 +3228,7 @@
         <xdr:cNvPr id="51" name="Conector recto 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000033000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3380,7 +3278,7 @@
         <xdr:cNvPr id="53" name="Conector recto 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3430,7 +3328,7 @@
         <xdr:cNvPr id="55" name="Conector recto 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3480,7 +3378,7 @@
         <xdr:cNvPr id="56" name="Conector recto 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3530,7 +3428,7 @@
         <xdr:cNvPr id="59" name="Conector recto 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3580,7 +3478,7 @@
         <xdr:cNvPr id="61" name="Conector recto 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3630,7 +3528,7 @@
         <xdr:cNvPr id="63" name="Conector recto 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3680,7 +3578,7 @@
         <xdr:cNvPr id="66" name="Conector recto 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3730,7 +3628,7 @@
         <xdr:cNvPr id="68" name="Conector recto 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000044000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3780,7 +3678,7 @@
         <xdr:cNvPr id="71" name="Conector recto 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3830,7 +3728,7 @@
         <xdr:cNvPr id="73" name="Conector recto 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000049000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3880,7 +3778,7 @@
         <xdr:cNvPr id="74" name="Conector recto 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00004A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3930,7 +3828,7 @@
         <xdr:cNvPr id="76" name="Conector recto 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00004C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3980,7 +3878,7 @@
         <xdr:cNvPr id="81" name="Conector recto 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000051000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4030,7 +3928,7 @@
         <xdr:cNvPr id="82" name="Conector recto 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4080,7 +3978,7 @@
         <xdr:cNvPr id="86" name="Conector recto 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000056000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4130,7 +4028,7 @@
         <xdr:cNvPr id="87" name="Conector recto 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000057000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4180,7 +4078,7 @@
         <xdr:cNvPr id="90" name="Conector recto 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4230,7 +4128,7 @@
         <xdr:cNvPr id="91" name="Conector recto 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00005B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4280,7 +4178,7 @@
         <xdr:cNvPr id="92" name="Conector recto 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00005C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4330,7 +4228,7 @@
         <xdr:cNvPr id="93" name="Conector recto 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00005D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4380,7 +4278,7 @@
         <xdr:cNvPr id="100" name="Conector recto 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000064000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000064000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4430,7 +4328,7 @@
         <xdr:cNvPr id="101" name="Conector recto 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000065000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4480,7 +4378,7 @@
         <xdr:cNvPr id="106" name="Conector recto 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00006A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4530,7 +4428,7 @@
         <xdr:cNvPr id="108" name="Conector recto 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4580,7 +4478,7 @@
         <xdr:cNvPr id="109" name="Conector recto 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00006D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4630,7 +4528,7 @@
         <xdr:cNvPr id="111" name="Conector recto 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00006F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4680,7 +4578,7 @@
         <xdr:cNvPr id="114" name="Conector recto 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000072000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4730,7 +4628,7 @@
         <xdr:cNvPr id="116" name="Conector recto 115">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000074000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000074000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4780,7 +4678,7 @@
         <xdr:cNvPr id="128" name="Conector recto 127">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000080000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4830,7 +4728,7 @@
         <xdr:cNvPr id="130" name="Conector recto 129">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000082000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4880,7 +4778,7 @@
         <xdr:cNvPr id="131" name="Conector recto 130">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000083000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4930,7 +4828,7 @@
         <xdr:cNvPr id="132" name="Conector recto 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000084000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4980,7 +4878,7 @@
         <xdr:cNvPr id="133" name="Conector recto 132">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000085000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000085000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5030,7 +4928,7 @@
         <xdr:cNvPr id="136" name="Conector recto 135">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000088000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000088000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5080,7 +4978,7 @@
         <xdr:cNvPr id="139" name="Conector recto 138">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5130,7 +5028,7 @@
         <xdr:cNvPr id="141" name="Conector recto 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5180,7 +5078,7 @@
         <xdr:cNvPr id="142" name="Conector recto 141">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5230,7 +5128,7 @@
         <xdr:cNvPr id="143" name="Conector recto 142">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00008F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5554,18 +5452,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView topLeftCell="L2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5624,13 +5522,13 @@
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="R3" s="131" t="s">
-        <v>185</v>
-      </c>
-      <c r="S3" s="132" t="s">
+      <c r="R3" s="124" t="s">
+        <v>184</v>
+      </c>
+      <c r="S3" s="125" t="s">
         <v>154</v>
       </c>
-      <c r="T3" s="132" t="s">
+      <c r="T3" s="125" t="s">
         <v>155</v>
       </c>
     </row>
@@ -5659,11 +5557,11 @@
       <c r="P4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="R4" s="133" t="s">
+      <c r="R4" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="S4" s="134"/>
-      <c r="T4" s="134"/>
+      <c r="S4" s="127"/>
+      <c r="T4" s="127"/>
     </row>
     <row r="5" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="47" t="s">
@@ -5687,11 +5585,11 @@
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
-      <c r="R5" s="133" t="s">
+      <c r="R5" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="S5" s="134"/>
-      <c r="T5" s="134"/>
+      <c r="S5" s="127"/>
+      <c r="T5" s="127"/>
     </row>
     <row r="6" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="47" t="s">
@@ -5713,11 +5611,11 @@
       </c>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
-      <c r="R6" s="135" t="s">
+      <c r="R6" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="136"/>
-      <c r="T6" s="136"/>
+      <c r="S6" s="129"/>
+      <c r="T6" s="129"/>
     </row>
     <row r="7" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="47" t="s">
@@ -5739,20 +5637,20 @@
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="R7" s="135" t="s">
+      <c r="R7" s="128" t="s">
         <v>156</v>
       </c>
-      <c r="S7" s="136"/>
-      <c r="T7" s="136"/>
+      <c r="S7" s="129"/>
+      <c r="T7" s="129"/>
     </row>
     <row r="8" spans="2:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="124" t="s">
-        <v>181</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="125"/>
+      <c r="B8" s="116" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="118" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="118"/>
       <c r="E8" s="3"/>
       <c r="J8" s="57" t="s">
         <v>4</v>
@@ -5764,20 +5662,20 @@
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="R8" s="135" t="s">
+      <c r="R8" s="128" t="s">
         <v>130</v>
       </c>
-      <c r="S8" s="136"/>
-      <c r="T8" s="136"/>
+      <c r="S8" s="129"/>
+      <c r="T8" s="129"/>
     </row>
     <row r="9" spans="2:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="126" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="121" t="s">
+      <c r="B9" s="119" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="121" t="s">
+      <c r="D9" s="117" t="s">
         <v>106</v>
       </c>
       <c r="E9" s="3"/>
@@ -5791,20 +5689,20 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="R9" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="S9" s="136"/>
-      <c r="T9" s="136"/>
+      <c r="R9" s="128" t="s">
+        <v>185</v>
+      </c>
+      <c r="S9" s="129"/>
+      <c r="T9" s="129"/>
     </row>
     <row r="10" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="117" t="s">
         <v>180</v>
       </c>
-      <c r="D10" s="121" t="s">
+      <c r="D10" s="117" t="s">
         <v>94</v>
       </c>
       <c r="E10" s="3"/>
@@ -5814,31 +5712,31 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="R10" s="135" t="s">
+      <c r="R10" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="S10" s="136"/>
-      <c r="T10" s="136"/>
+      <c r="S10" s="129"/>
+      <c r="T10" s="129"/>
     </row>
     <row r="11" spans="2:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="127" t="s">
+      <c r="B11" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="121" t="s">
         <v>180</v>
       </c>
-      <c r="D11" s="129" t="s">
+      <c r="D11" s="122" t="s">
         <v>94</v>
       </c>
       <c r="E11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="R11" s="137" t="s">
+      <c r="R11" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="S11" s="138"/>
-      <c r="T11" s="138"/>
+      <c r="S11" s="131"/>
+      <c r="T11" s="131"/>
     </row>
     <row r="12" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="38"/>
@@ -5889,7 +5787,7 @@
       <c r="M15" s="4"/>
       <c r="P15" s="27"/>
       <c r="R15" s="45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="S15" s="10" t="s">
         <v>154</v>
@@ -5919,7 +5817,7 @@
       <c r="I17" s="3"/>
       <c r="M17" s="3"/>
       <c r="R17" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
@@ -5967,7 +5865,7 @@
       <c r="L20" s="9"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="47" t="s">
@@ -5979,6 +5877,9 @@
       <c r="Q21" s="23"/>
     </row>
     <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="51" t="s">
+        <v>85</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="47" t="s">
@@ -5992,8 +5893,8 @@
       <c r="A23" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>15</v>
+      <c r="B23" s="45" t="s">
+        <v>22</v>
       </c>
       <c r="E23" s="3"/>
       <c r="I23" s="3"/>
@@ -6066,9 +5967,6 @@
       <c r="A28" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="51" t="s">
-        <v>84</v>
-      </c>
       <c r="E28" s="3"/>
       <c r="F28" s="51" t="s">
         <v>21</v>
@@ -6095,8 +5993,8 @@
       <c r="A29" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="45" t="s">
-        <v>30</v>
+      <c r="B29" s="51" t="s">
+        <v>84</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="46" t="s">
@@ -6126,7 +6024,7 @@
         <v>110</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F30" s="46" t="s">
         <v>132</v>
@@ -6139,7 +6037,7 @@
       <c r="J30" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="121" t="s">
+      <c r="K30" s="117" t="s">
         <v>180</v>
       </c>
       <c r="L30" s="1" t="s">
@@ -6162,10 +6060,10 @@
         <v>107</v>
       </c>
       <c r="H31" s="55"/>
-      <c r="J31" s="127" t="s">
+      <c r="J31" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="K31" s="121" t="s">
+      <c r="K31" s="117" t="s">
         <v>180</v>
       </c>
       <c r="L31" s="2" t="s">
@@ -6383,23 +6281,14 @@
       <c r="L45" s="2"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F47" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>101</v>
-      </c>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -6407,111 +6296,70 @@
       <c r="M47" s="3"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F48" s="116" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="117" t="s">
-        <v>107</v>
-      </c>
-      <c r="H48" s="118" t="s">
-        <v>103</v>
-      </c>
       <c r="I48" s="43"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F49" s="119" t="s">
-        <v>130</v>
-      </c>
-      <c r="G49" s="89" t="s">
-        <v>140</v>
-      </c>
-      <c r="H49" s="120"/>
+    <row r="49" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I49" s="43"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F50" s="119" t="s">
-        <v>131</v>
-      </c>
-      <c r="G50" s="117" t="s">
-        <v>107</v>
-      </c>
-      <c r="H50" s="120"/>
+    <row r="50" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I50" s="43"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F51" s="119" t="s">
-        <v>4</v>
-      </c>
-      <c r="G51" s="121" t="s">
-        <v>180</v>
-      </c>
-      <c r="H51" s="120" t="s">
-        <v>94</v>
-      </c>
+    <row r="51" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I51" s="43"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F52" s="122" t="s">
-        <v>3</v>
-      </c>
-      <c r="G52" s="121" t="s">
-        <v>180</v>
-      </c>
-      <c r="H52" s="123" t="s">
-        <v>94</v>
-      </c>
+    <row r="52" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I52" s="44"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M54" s="4"/>
     </row>
-    <row r="55" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:13" x14ac:dyDescent="0.25">
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="62" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="6:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M64" s="3"/>
     </row>
     <row r="65" spans="13:13" x14ac:dyDescent="0.25">
@@ -6531,10 +6379,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+    <sheetView topLeftCell="A95" workbookViewId="0">
       <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
@@ -8119,7 +7967,7 @@
         <v>157</v>
       </c>
       <c r="G79" s="115" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H79" s="64" t="s">
         <v>4</v>
@@ -8173,7 +8021,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B82" s="47"/>
       <c r="C82" s="1"/>
@@ -8331,7 +8179,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="104" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B91" s="105"/>
       <c r="C91" s="106"/>
@@ -8414,7 +8262,7 @@
         <v>168</v>
       </c>
       <c r="J95" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K95" s="63" t="s">
         <v>4</v>
@@ -8546,7 +8394,7 @@
         <v>168</v>
       </c>
       <c r="B100" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C100" s="21" t="s">
         <v>94</v>
@@ -8574,10 +8422,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B101" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J101" s="3"/>
     </row>
@@ -8617,7 +8465,7 @@
     </row>
     <row r="106" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B106" s="10" t="s">
         <v>154</v>
@@ -8629,13 +8477,13 @@
         <v>23</v>
       </c>
       <c r="F106" s="112" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G106" s="112" t="s">
+        <v>190</v>
+      </c>
+      <c r="H106" s="63" t="s">
         <v>191</v>
-      </c>
-      <c r="H106" s="63" t="s">
-        <v>192</v>
       </c>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
@@ -8650,13 +8498,13 @@
         <v>107</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E107" s="65">
         <v>0</v>
       </c>
       <c r="F107" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G107" s="113"/>
       <c r="H107" s="21">
@@ -8669,8 +8517,8 @@
       <c r="M107" s="3"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A108" s="130" t="s">
-        <v>187</v>
+      <c r="A108" s="123" t="s">
+        <v>186</v>
       </c>
       <c r="B108" s="9" t="s">
         <v>140</v>
@@ -8680,7 +8528,7 @@
         <v>1</v>
       </c>
       <c r="F108" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G108" s="113"/>
       <c r="H108" s="21">
@@ -8711,11 +8559,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G96" r:id="rId1"/>
-    <hyperlink ref="G97" r:id="rId2"/>
-    <hyperlink ref="G98" r:id="rId3"/>
-    <hyperlink ref="G99" r:id="rId4"/>
-    <hyperlink ref="G100" r:id="rId5"/>
+    <hyperlink ref="G96" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G97" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G98" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G99" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G100" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -8724,7 +8572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:L89"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
@@ -9870,7 +9718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -10301,7 +10149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>